<commit_message>
deleted clap detection, changed hardware to version 01 (round pcb)
</commit_message>
<xml_diff>
--- a/0_Documentation/Modbus/ModbusMod.xlsx
+++ b/0_Documentation/Modbus/ModbusMod.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="359">
   <si>
     <t>BIT15</t>
   </si>
@@ -972,9 +972,6 @@
     <t>SOUND_MV</t>
   </si>
   <si>
-    <t>SOUND_CLAPCOUNT</t>
-  </si>
-  <si>
     <t>THTIM_15</t>
   </si>
   <si>
@@ -1059,52 +1056,52 @@
     <t>SOUND0</t>
   </si>
   <si>
-    <t>CLCNT15</t>
-  </si>
-  <si>
-    <t>CLCNT14</t>
-  </si>
-  <si>
-    <t>CLCNT13</t>
-  </si>
-  <si>
-    <t>CLCNT12</t>
-  </si>
-  <si>
-    <t>CLCNT11</t>
-  </si>
-  <si>
-    <t>CLCNT10</t>
-  </si>
-  <si>
-    <t>CLCNT9</t>
-  </si>
-  <si>
-    <t>CLCNT8</t>
-  </si>
-  <si>
-    <t>CLCNT7</t>
-  </si>
-  <si>
-    <t>CLCNT6</t>
-  </si>
-  <si>
-    <t>CLCNT5</t>
-  </si>
-  <si>
-    <t>CLCNT4</t>
-  </si>
-  <si>
-    <t>CLCNT3</t>
-  </si>
-  <si>
-    <t>CLCNT2</t>
-  </si>
-  <si>
-    <t>CLCNT1</t>
-  </si>
-  <si>
-    <t>CLCNT0</t>
+    <t>SOUNDPERC0</t>
+  </si>
+  <si>
+    <t>SOUNDPERC1</t>
+  </si>
+  <si>
+    <t>SOUNDPERC6</t>
+  </si>
+  <si>
+    <t>SOUNDPERC5</t>
+  </si>
+  <si>
+    <t>SOUNDPERC4</t>
+  </si>
+  <si>
+    <t>SOUNDPERC3</t>
+  </si>
+  <si>
+    <t>SOUNDPERC2</t>
+  </si>
+  <si>
+    <t>PIRCOUNT7</t>
+  </si>
+  <si>
+    <t>PIRCOUNT6</t>
+  </si>
+  <si>
+    <t>PIRCOUNT5</t>
+  </si>
+  <si>
+    <t>PIRCOUNT4</t>
+  </si>
+  <si>
+    <t>PIRCOUNT3</t>
+  </si>
+  <si>
+    <t>PIRCOUNT2</t>
+  </si>
+  <si>
+    <t>PIRCOUNT1</t>
+  </si>
+  <si>
+    <t>PIRCOUNT0</t>
+  </si>
+  <si>
+    <t>FAST_PIRCOUNT_SOUNDPERCENT</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1466,7 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,6 +1604,33 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>45</v>
+      </c>
       <c r="L3" t="s">
         <v>276</v>
       </c>
@@ -2589,52 +2613,52 @@
         <v>313</v>
       </c>
       <c r="C21" t="s">
+        <v>315</v>
+      </c>
+      <c r="D21" t="s">
         <v>316</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>317</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>318</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>319</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>320</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>321</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>322</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>323</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>324</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>325</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>326</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>327</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>328</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>329</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>330</v>
-      </c>
-      <c r="R21" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2657,40 +2681,40 @@
         <v>81</v>
       </c>
       <c r="G22" t="s">
+        <v>331</v>
+      </c>
+      <c r="H22" t="s">
         <v>332</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>333</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>334</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>335</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>336</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>337</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>338</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>339</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>340</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>341</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>342</v>
-      </c>
-      <c r="R22" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2698,55 +2722,55 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>315</v>
+        <v>358</v>
       </c>
       <c r="C23" t="s">
+        <v>350</v>
+      </c>
+      <c r="D23" t="s">
+        <v>351</v>
+      </c>
+      <c r="E23" t="s">
+        <v>352</v>
+      </c>
+      <c r="F23" t="s">
+        <v>353</v>
+      </c>
+      <c r="G23" t="s">
+        <v>354</v>
+      </c>
+      <c r="H23" t="s">
+        <v>355</v>
+      </c>
+      <c r="I23" t="s">
+        <v>356</v>
+      </c>
+      <c r="J23" t="s">
+        <v>357</v>
+      </c>
+      <c r="K23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L23" t="s">
+        <v>345</v>
+      </c>
+      <c r="M23" t="s">
+        <v>346</v>
+      </c>
+      <c r="N23" t="s">
+        <v>347</v>
+      </c>
+      <c r="O23" t="s">
+        <v>348</v>
+      </c>
+      <c r="P23" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q23" t="s">
         <v>344</v>
       </c>
-      <c r="D23" t="s">
-        <v>345</v>
-      </c>
-      <c r="E23" t="s">
-        <v>346</v>
-      </c>
-      <c r="F23" t="s">
-        <v>347</v>
-      </c>
-      <c r="G23" t="s">
-        <v>348</v>
-      </c>
-      <c r="H23" t="s">
-        <v>349</v>
-      </c>
-      <c r="I23" t="s">
-        <v>350</v>
-      </c>
-      <c r="J23" t="s">
-        <v>351</v>
-      </c>
-      <c r="K23" t="s">
-        <v>352</v>
-      </c>
-      <c r="L23" t="s">
-        <v>353</v>
-      </c>
-      <c r="M23" t="s">
-        <v>354</v>
-      </c>
-      <c r="N23" t="s">
-        <v>355</v>
-      </c>
-      <c r="O23" t="s">
-        <v>356</v>
-      </c>
-      <c r="P23" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>358</v>
-      </c>
       <c r="R23" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>